<commit_message>
refactor : application.yaml 파일 h2,mysql 분리
application.yaml 파일 h2,mysql 분리
</commit_message>
<xml_diff>
--- a/Library 프로젝트 요구사항 정의서.xlsx
+++ b/Library 프로젝트 요구사항 정의서.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\library project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
   <si>
     <t>요구사항 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -389,6 +389,103 @@
   <si>
     <t>PUBLISHER 를 포함한 GET 요청을 통해 
 특정 출판사의 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_002</t>
+  </si>
+  <si>
+    <t>SECURITY_003</t>
+  </si>
+  <si>
+    <t>SECURITY_004</t>
+  </si>
+  <si>
+    <t>SECURITY_FORM_LOGIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_005</t>
+  </si>
+  <si>
+    <t>SECURITY_006</t>
+  </si>
+  <si>
+    <t>SECURITY_KAKAO_LOGIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_GOOGLE_LOGIN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_JWT_TOKEN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_REFRESH_TOKEN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_LOGOUT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOGINDTO.POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY_007</t>
+  </si>
+  <si>
+    <t>SECURITY_PASSWORD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 SIGN_IN시 사용한 ID 와 PASSWORD 로 인증 및 인가 받을 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 KAKAO OAUTH2 기능을 이용하여 자동 회원가입 및 로그인을 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 GOOGLE OAUTH2 기능을 이용하여 자동 회원가입 및 로그인을 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증 및 인가는 백엔드 서버에서 생성한 JWT 를 이용하여 진행된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 REFRESH TOKEN 을 사용하여 ACESS TOKEN 을 재발급 받을 수 있다.
+단, REFRESH TOKEN 의 만료시간 전에만 받을 수 있고, 
+LOGOUT 시에는 REFRESH TOKEN 은 삭제된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자는 원하는 시간에 LOGOUT을 진행하여 REFRESH TOKEN을 삭제할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자의 PASSWORD DATA 는 
+SIGN_IN 이후 PASSWORD_ENCODER 로 암호화하여 통신한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -462,7 +559,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -483,15 +580,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -528,13 +616,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -817,17 +905,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="58.25" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.4140625" customWidth="1"/>
     <col min="4" max="4" width="21.58203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
@@ -1058,10 +1146,10 @@
       <c r="A15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
@@ -1149,13 +1237,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="17" customHeight="1">
       <c r="A22" s="5" t="s">
@@ -1268,8 +1356,137 @@
         <v>24</v>
       </c>
     </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" ht="34">
+      <c r="A30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="68">
+      <c r="A35" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A15:E15"/>

</xml_diff>